<commit_message>
Adding Agent and Admin
</commit_message>
<xml_diff>
--- a/Controller/Ticket_Details.xlsx
+++ b/Controller/Ticket_Details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>ticketID</t>
   </si>
@@ -53,22 +53,91 @@
     <t>Close</t>
   </si>
   <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>2023-11-28 19:17:00</t>
+  </si>
+  <si>
+    <t>2023-12-05 15:28:00</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>sdfghjkjhgfc</t>
+  </si>
+  <si>
+    <t>asdfg</t>
+  </si>
+  <si>
+    <t>2023-12-13 12:45:00</t>
+  </si>
+  <si>
+    <t>aasdfgbvc</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>2023-11-29 17:07:00</t>
+  </si>
+  <si>
+    <t>2023-12-07 15:45:00</t>
+  </si>
+  <si>
+    <t>asdcfvbnm,.,mnbvc</t>
+  </si>
+  <si>
+    <t>asdfghnjk,mnbv</t>
+  </si>
+  <si>
+    <t>2023-11-29 17:12:00</t>
+  </si>
+  <si>
+    <t>2023-12-19 11:45:00</t>
+  </si>
+  <si>
+    <t>sdfghjkllvcx</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
     <t>high</t>
   </si>
   <si>
-    <t>2023-12-07 14:56:00</t>
-  </si>
-  <si>
-    <t>2023-12-19 13:51:00</t>
-  </si>
-  <si>
-    <t>Nothing</t>
-  </si>
-  <si>
-    <t>asdfghjkjhgfds</t>
-  </si>
-  <si>
-    <t>xcvnmnbvc</t>
+    <t>2023-12-10 17:16:00</t>
+  </si>
+  <si>
+    <t>2023-12-10 17:16:33</t>
+  </si>
+  <si>
+    <t>Online Banking</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:06:00</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:06:38</t>
+  </si>
+  <si>
+    <t>asdfghjkl</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:36:00</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:36:29</t>
+  </si>
+  <si>
+    <t>QWRTYUH</t>
+  </si>
+  <si>
+    <t>asdfghjkl;</t>
   </si>
   <si>
     <t>2023-12-17 16:54:00</t>
@@ -77,10 +146,49 @@
     <t>2023-12-18 14:27:00</t>
   </si>
   <si>
-    <t>asdfghjkl</t>
-  </si>
-  <si>
-    <t>Done</t>
+    <t>2023-12-17 16:55:00</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:55:36</t>
+  </si>
+  <si>
+    <t>asdrtfyuio</t>
+  </si>
+  <si>
+    <t>2023-12-18 14:25:00</t>
+  </si>
+  <si>
+    <t>2023-12-18 14:25:29</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum</t>
+  </si>
+  <si>
+    <t>2023-12-18 14:26:00</t>
+  </si>
+  <si>
+    <t>2023-12-18 14:26:29</t>
+  </si>
+  <si>
+    <t>2023-12-19 11:45:22</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>2023-12-19 15:48:00</t>
+  </si>
+  <si>
+    <t>2023-12-19 15:48:57</t>
+  </si>
+  <si>
+    <t>2023-12-19 15:52:00</t>
+  </si>
+  <si>
+    <t>2023-12-19 15:52:37</t>
+  </si>
+  <si>
+    <t>asdfghjklkjhgfdewqw34r567890</t>
   </si>
 </sst>
 </file>
@@ -420,7 +528,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +573,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -492,7 +600,7 @@
         <v>301</v>
       </c>
       <c r="J2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
         <v>17</v>
@@ -500,7 +608,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -509,28 +617,421 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
+        <v>301</v>
+      </c>
+      <c r="J3">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>302</v>
+      </c>
+      <c r="J4">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>303</v>
+      </c>
+      <c r="J5">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>303</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>325</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
         <v>308</v>
       </c>
-      <c r="J3">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>308</v>
+      </c>
+      <c r="J9">
         <v>45</v>
       </c>
-      <c r="K3" t="s">
-        <v>21</v>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>93</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>305</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>324</v>
+      </c>
+      <c r="J11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>303</v>
+      </c>
+      <c r="J12">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <v>324</v>
+      </c>
+      <c r="J13">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>301</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>301</v>
+      </c>
+      <c r="J15">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploading client related files
</commit_message>
<xml_diff>
--- a/Controller/Ticket_Details.xlsx
+++ b/Controller/Ticket_Details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>ticketID</t>
   </si>
@@ -50,136 +50,100 @@
     <t>remarks</t>
   </si>
   <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>2023-12-10 17:16:00</t>
+  </si>
+  <si>
+    <t>2023-12-10 17:16:33</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>Online Banking</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:06:00</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:06:38</t>
+  </si>
+  <si>
+    <t>asdfghjkl</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:36:00</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:36:29</t>
+  </si>
+  <si>
+    <t>QWRTYUH</t>
+  </si>
+  <si>
+    <t>asdfghjkl;</t>
+  </si>
+  <si>
     <t>Close</t>
   </si>
   <si>
+    <t>2023-12-17 16:54:00</t>
+  </si>
+  <si>
+    <t>2023-12-18 14:27:00</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:55:00</t>
+  </si>
+  <si>
+    <t>2023-12-17 16:55:36</t>
+  </si>
+  <si>
+    <t>asdrtfyuio</t>
+  </si>
+  <si>
+    <t>2023-12-18 14:25:00</t>
+  </si>
+  <si>
+    <t>2023-12-18 14:25:29</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum</t>
+  </si>
+  <si>
+    <t>2023-12-18 14:26:00</t>
+  </si>
+  <si>
+    <t>2023-12-18 14:26:29</t>
+  </si>
+  <si>
+    <t>2023-12-19 11:45:00</t>
+  </si>
+  <si>
+    <t>2023-12-19 11:45:22</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>2023-12-19 15:48:00</t>
+  </si>
+  <si>
+    <t>2023-12-19 15:48:57</t>
+  </si>
+  <si>
     <t>medium</t>
-  </si>
-  <si>
-    <t>2023-11-28 19:17:00</t>
-  </si>
-  <si>
-    <t>2023-12-05 15:28:00</t>
-  </si>
-  <si>
-    <t>Nothing</t>
-  </si>
-  <si>
-    <t>sdfghjkjhgfc</t>
-  </si>
-  <si>
-    <t>asdfg</t>
-  </si>
-  <si>
-    <t>2023-12-13 12:45:00</t>
-  </si>
-  <si>
-    <t>aasdfgbvc</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>2023-11-29 17:07:00</t>
-  </si>
-  <si>
-    <t>2023-12-07 15:45:00</t>
-  </si>
-  <si>
-    <t>asdcfvbnm,.,mnbvc</t>
-  </si>
-  <si>
-    <t>asdfghnjk,mnbv</t>
-  </si>
-  <si>
-    <t>2023-11-29 17:12:00</t>
-  </si>
-  <si>
-    <t>2023-12-19 11:45:00</t>
-  </si>
-  <si>
-    <t>sdfghjkllvcx</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>2023-12-10 17:16:00</t>
-  </si>
-  <si>
-    <t>2023-12-10 17:16:33</t>
-  </si>
-  <si>
-    <t>Online Banking</t>
-  </si>
-  <si>
-    <t>2023-12-17 16:06:00</t>
-  </si>
-  <si>
-    <t>2023-12-17 16:06:38</t>
-  </si>
-  <si>
-    <t>asdfghjkl</t>
-  </si>
-  <si>
-    <t>2023-12-17 16:36:00</t>
-  </si>
-  <si>
-    <t>2023-12-17 16:36:29</t>
-  </si>
-  <si>
-    <t>QWRTYUH</t>
-  </si>
-  <si>
-    <t>asdfghjkl;</t>
-  </si>
-  <si>
-    <t>2023-12-17 16:54:00</t>
-  </si>
-  <si>
-    <t>2023-12-18 14:27:00</t>
-  </si>
-  <si>
-    <t>2023-12-17 16:55:00</t>
-  </si>
-  <si>
-    <t>2023-12-17 16:55:36</t>
-  </si>
-  <si>
-    <t>asdrtfyuio</t>
-  </si>
-  <si>
-    <t>2023-12-18 14:25:00</t>
-  </si>
-  <si>
-    <t>2023-12-18 14:25:29</t>
-  </si>
-  <si>
-    <t>Lorem Ipsum</t>
-  </si>
-  <si>
-    <t>2023-12-18 14:26:00</t>
-  </si>
-  <si>
-    <t>2023-12-18 14:26:29</t>
-  </si>
-  <si>
-    <t>2023-12-19 11:45:22</t>
-  </si>
-  <si>
-    <t>Updated</t>
-  </si>
-  <si>
-    <t>2023-12-19 15:48:00</t>
-  </si>
-  <si>
-    <t>2023-12-19 15:48:57</t>
   </si>
   <si>
     <t>2023-12-19 15:52:00</t>
@@ -528,7 +492,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +537,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -594,21 +558,18 @@
         <v>16</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J2">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -617,7 +578,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -626,62 +587,56 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I3">
-        <v>301</v>
+        <v>325</v>
       </c>
       <c r="J3">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="J4">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -696,179 +651,176 @@
         <v>15</v>
       </c>
       <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>308</v>
+      </c>
+      <c r="J5">
+        <v>45</v>
+      </c>
+      <c r="K5" t="s">
         <v>27</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>303</v>
-      </c>
-      <c r="J5">
-        <v>25</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
       <c r="H6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="J6">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I7">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I8">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I9">
-        <v>308</v>
+        <v>324</v>
       </c>
       <c r="J9">
-        <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -876,161 +828,33 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I11">
-        <v>324</v>
+        <v>301</v>
       </c>
       <c r="J11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12">
-        <v>95</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12">
-        <v>8</v>
-      </c>
-      <c r="I12">
-        <v>303</v>
-      </c>
-      <c r="J12">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13">
-        <v>96</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13">
-        <v>7</v>
-      </c>
-      <c r="I13">
-        <v>324</v>
-      </c>
-      <c r="J13">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14">
-        <v>97</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <v>301</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15">
-        <v>98</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>301</v>
-      </c>
-      <c r="J15">
         <v>49</v>
       </c>
     </row>

</xml_diff>